<commit_message>
Updates to coding system and case matrix
</commit_message>
<xml_diff>
--- a/case-characterization-matrix.xlsx
+++ b/case-characterization-matrix.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspace\phd\research-microservices-evolvability-interviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E65C6E-0D98-414C-8C28-45F380DDDFEB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5CFEB1-98E5-494A-9670-D60B84E95892}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company Demographics" sheetId="3" r:id="rId1"/>
     <sheet name="Systems and Assurance Processes" sheetId="1" r:id="rId2"/>
+    <sheet name="Assurance Reflection Chart" sheetId="4" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Systems and Assurance Processes'!$A$1:$M$18</definedName>
   </definedNames>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="139">
   <si>
     <t>Participant ID</t>
   </si>
@@ -310,10 +314,6 @@
 Impact (-2 to +2)</t>
   </si>
   <si>
-    <t>Wanted Change for 
-Assurance Efforts (-2 to +2)</t>
-  </si>
-  <si>
     <t>System
 ID</t>
   </si>
@@ -430,6 +430,37 @@
   </si>
   <si>
     <t>Event-Driven Messaging, Self-Contained Systems, Event Sourcing</t>
+  </si>
+  <si>
+    <t>Very negative (-2)</t>
+  </si>
+  <si>
+    <t>Negative (-1)</t>
+  </si>
+  <si>
+    <t>Neutral (0)</t>
+  </si>
+  <si>
+    <t>Positive (+1)</t>
+  </si>
+  <si>
+    <t>Very Positive (+2)</t>
+  </si>
+  <si>
+    <t>Evolvability Rating</t>
+  </si>
+  <si>
+    <t>Assurance Effectiveness</t>
+  </si>
+  <si>
+    <t>Assurance Impact on Productivity</t>
+  </si>
+  <si>
+    <t>Wanted Change in Assurance Efforts</t>
+  </si>
+  <si>
+    <t>Wanted Change in 
+Assurance Efforts (-2 to +2)</t>
   </si>
 </sst>
 </file>
@@ -502,7 +533,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -556,6 +587,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -566,11 +601,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -583,9 +618,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -603,6 +635,1521 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Assurance Reflection Chart'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Very negative (-2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Assurance Reflection Chart'!$A$3:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Wanted Change in Assurance Efforts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Assurance Impact on Productivity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Assurance Effectiveness</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Evolvability Rating</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Assurance Reflection Chart'!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F240-4BC1-BBA1-6456F793EA3A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Assurance Reflection Chart'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Negative (-1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-F240-4BC1-BBA1-6456F793EA3A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Assurance Reflection Chart'!$A$3:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Wanted Change in Assurance Efforts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Assurance Impact on Productivity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Assurance Effectiveness</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Evolvability Rating</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Assurance Reflection Chart'!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F240-4BC1-BBA1-6456F793EA3A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Assurance Reflection Chart'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Neutral (0)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Assurance Reflection Chart'!$A$3:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Wanted Change in Assurance Efforts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Assurance Impact on Productivity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Assurance Effectiveness</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Evolvability Rating</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Assurance Reflection Chart'!$D$3:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F240-4BC1-BBA1-6456F793EA3A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Assurance Reflection Chart'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Positive (+1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Assurance Reflection Chart'!$A$3:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Wanted Change in Assurance Efforts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Assurance Impact on Productivity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Assurance Effectiveness</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Evolvability Rating</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Assurance Reflection Chart'!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F240-4BC1-BBA1-6456F793EA3A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Assurance Reflection Chart'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Very Positive (+2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Assurance Reflection Chart'!$A$3:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Wanted Change in Assurance Efforts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Assurance Impact on Productivity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Assurance Effectiveness</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Evolvability Rating</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Assurance Reflection Chart'!$F$3:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F240-4BC1-BBA1-6456F793EA3A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="792734272"/>
+        <c:axId val="792729920"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="792734272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="792729920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="792729920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="792734272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1100" b="1">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47627</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17A0A90D-D7EE-49E8-BC16-EA43CD246CD7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="metrics"/>
+      <sheetName val="experiment"/>
+      <sheetName val="survey"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2">
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>Strongly Disagree</v>
+          </cell>
+          <cell r="C2" t="str">
+            <v>Disagree</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>Neutral</v>
+          </cell>
+          <cell r="E2" t="str">
+            <v>Agree</v>
+          </cell>
+          <cell r="F2" t="str">
+            <v>Strongly Agree</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>Service Orientation</v>
+          </cell>
+          <cell r="B3">
+            <v>0</v>
+          </cell>
+          <cell r="C3">
+            <v>2</v>
+          </cell>
+          <cell r="D3">
+            <v>4</v>
+          </cell>
+          <cell r="E3">
+            <v>20</v>
+          </cell>
+          <cell r="F3">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Object Orientation</v>
+          </cell>
+          <cell r="B4">
+            <v>1</v>
+          </cell>
+          <cell r="C4">
+            <v>7</v>
+          </cell>
+          <cell r="D4">
+            <v>8</v>
+          </cell>
+          <cell r="E4">
+            <v>15</v>
+          </cell>
+          <cell r="F4">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17" t="str">
+            <v>Strongly Disagree</v>
+          </cell>
+          <cell r="C17" t="str">
+            <v>Disagree</v>
+          </cell>
+          <cell r="D17" t="str">
+            <v>Neutral</v>
+          </cell>
+          <cell r="E17" t="str">
+            <v>Agree</v>
+          </cell>
+          <cell r="F17" t="str">
+            <v>Strongly Agree</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>Service Orientation</v>
+          </cell>
+          <cell r="B18">
+            <v>0</v>
+          </cell>
+          <cell r="C18">
+            <v>3</v>
+          </cell>
+          <cell r="D18">
+            <v>4</v>
+          </cell>
+          <cell r="E18">
+            <v>22</v>
+          </cell>
+          <cell r="F18">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>Object Orientation</v>
+          </cell>
+          <cell r="B19">
+            <v>0</v>
+          </cell>
+          <cell r="C19">
+            <v>1</v>
+          </cell>
+          <cell r="D19">
+            <v>12</v>
+          </cell>
+          <cell r="E19">
+            <v>15</v>
+          </cell>
+          <cell r="F19">
+            <v>4</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -904,9 +2451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9F47F6-107E-4EC3-AB9A-0F0222BB4338}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -966,13 +2511,13 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="24" t="s">
         <v>73</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -989,9 +2534,9 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="4" t="s">
         <v>48</v>
       </c>
@@ -1006,9 +2551,9 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="4" t="s">
         <v>49</v>
       </c>
@@ -1023,13 +2568,13 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="24" t="s">
         <v>74</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -1041,14 +2586,14 @@
       <c r="F6" s="3">
         <v>20</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="26" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="4" t="s">
         <v>51</v>
       </c>
@@ -1058,16 +2603,16 @@
       <c r="F7" s="3">
         <v>8</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="22"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="24" t="s">
         <v>68</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -1084,9 +2629,9 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="4" t="s">
         <v>53</v>
       </c>
@@ -1124,13 +2669,13 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="24" t="s">
         <v>66</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -1142,14 +2687,14 @@
       <c r="F11" s="3">
         <v>9</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="4" t="s">
         <v>56</v>
       </c>
@@ -1159,12 +2704,12 @@
       <c r="F12" s="3">
         <v>7</v>
       </c>
-      <c r="G12" s="20"/>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="4" t="s">
         <v>57</v>
       </c>
@@ -1179,13 +2724,13 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="24" t="s">
         <v>68</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -1202,9 +2747,9 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="4" t="s">
         <v>59</v>
       </c>
@@ -8163,12 +9708,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
@@ -8180,6 +9719,12 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup scale="45" orientation="landscape"/>
@@ -8190,7 +9735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -8214,21 +9759,21 @@
     <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="29" customFormat="1" ht="39.75" customHeight="1" thickBot="1">
+    <row r="1" spans="1:13" s="20" customFormat="1" ht="39.75" customHeight="1" thickBot="1">
       <c r="A1" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>93</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>94</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>5</v>
@@ -8252,7 +9797,7 @@
         <v>90</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1">
@@ -8272,13 +9817,13 @@
         <v>46</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>64</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I2" s="14">
         <v>2</v>
@@ -8316,10 +9861,10 @@
         <v>14</v>
       </c>
       <c r="G3" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>97</v>
       </c>
       <c r="I3" s="14">
         <v>3</v>
@@ -8357,10 +9902,10 @@
         <v>14</v>
       </c>
       <c r="G4" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>99</v>
       </c>
       <c r="I4" s="14">
         <v>1.5</v>
@@ -8395,13 +9940,13 @@
         <v>49</v>
       </c>
       <c r="F5" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>102</v>
       </c>
       <c r="I5" s="14">
         <v>1.5</v>
@@ -8420,29 +9965,29 @@
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="28">
         <v>7</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="30">
         <v>6</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="25" t="s">
-        <v>97</v>
+      <c r="H6" s="27" t="s">
+        <v>96</v>
       </c>
       <c r="I6" s="14">
         <v>1</v>
@@ -8461,16 +10006,16 @@
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="28"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
       <c r="I7" s="14">
         <v>1.5</v>
       </c>
@@ -8504,13 +10049,13 @@
         <v>52</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>105</v>
-      </c>
       <c r="H8" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I8" s="14">
         <v>3</v>
@@ -8545,13 +10090,13 @@
         <v>53</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I9" s="14">
         <v>2.5</v>
@@ -8586,13 +10131,13 @@
         <v>54</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I10" s="14">
         <v>2</v>
@@ -8611,29 +10156,29 @@
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="28" t="s">
         <v>84</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>55</v>
       </c>
       <c r="F11" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H11" s="25" t="s">
-        <v>114</v>
+      <c r="H11" s="27" t="s">
+        <v>113</v>
       </c>
       <c r="I11" s="14">
         <v>1.5</v>
@@ -8652,20 +10197,20 @@
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="26"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="13" t="s">
         <v>56</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="H12" s="25"/>
+        <v>112</v>
+      </c>
+      <c r="H12" s="27"/>
       <c r="I12" s="14">
         <v>3</v>
       </c>
@@ -8699,13 +10244,13 @@
         <v>57</v>
       </c>
       <c r="F13" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="H13" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="I13" s="14">
         <v>2</v>
@@ -8724,26 +10269,26 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="22" t="s">
-        <v>118</v>
+      <c r="D14" s="24" t="s">
+        <v>117</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>58</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H14" s="18" t="s">
         <v>64</v>
@@ -8765,18 +10310,18 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="30">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="22"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="13" t="s">
         <v>59</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H15" s="18" t="s">
         <v>64</v>
@@ -8814,13 +10359,13 @@
         <v>60</v>
       </c>
       <c r="F16" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="H16" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="I16" s="14">
         <v>2.5</v>
@@ -8858,10 +10403,10 @@
         <v>14</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I17" s="2">
         <v>2</v>
@@ -8896,13 +10441,13 @@
         <v>62</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="I18" s="2">
         <v>2</v>
@@ -9952,4 +11497,143 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D48F01DD-3580-42B6-BC61-08BBFF2D470E}">
+  <dimension ref="A2:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$M$2:$M$18, -2)</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$M$2:$M$18, -1)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$M$2:$M$18, 0)</f>
+        <v>7</v>
+      </c>
+      <c r="E3" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$M$2:$M$18, 1)</f>
+        <v>7</v>
+      </c>
+      <c r="F3" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$M$2:$M$18, 2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$L$2:$L$18, -2)</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$L$2:$L$18, -1)</f>
+        <v>3</v>
+      </c>
+      <c r="D4" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$L$2:$L$18, 0)</f>
+        <v>4</v>
+      </c>
+      <c r="E4" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$L$2:$L$18, 1)</f>
+        <v>7</v>
+      </c>
+      <c r="F4" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$L$2:$L$18, 2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$K$2:$K$18, -2)</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$K$2:$K$18, -1)</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$K$2:$K$18, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$K$2:$K$18, 1)</f>
+        <v>11</v>
+      </c>
+      <c r="F5" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$K$2:$K$18, 2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6">
+        <f>COUNTIF('Systems and Assurance Processes'!$J$2:$J$18, -2)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$J$2:$J$18, -1)</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$J$2:$J$18, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="E6" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$J$2:$J$18, 1)</f>
+        <v>9</v>
+      </c>
+      <c r="F6" s="19">
+        <f>COUNTIF('Systems and Assurance Processes'!$J$2:$J$18, 2)</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added medians to case matrix
</commit_message>
<xml_diff>
--- a/case-characterization-matrix.xlsx
+++ b/case-characterization-matrix.xlsx
@@ -8,18 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspace\phd\research-microservices-evolvability-interviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5CFEB1-98E5-494A-9670-D60B84E95892}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A41F633-1A2A-41F7-91A2-6673134911BE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company Demographics" sheetId="3" r:id="rId1"/>
     <sheet name="Systems and Assurance Processes" sheetId="1" r:id="rId2"/>
     <sheet name="Assurance Reflection Chart" sheetId="4" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Systems and Assurance Processes'!$A$1:$M$18</definedName>
   </definedNames>
@@ -35,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="140">
   <si>
     <t>Participant ID</t>
   </si>
@@ -461,6 +458,9 @@
   <si>
     <t>Wanted Change in 
 Assurance Efforts (-2 to +2)</t>
+  </si>
+  <si>
+    <t>Medians:</t>
   </si>
 </sst>
 </file>
@@ -601,11 +601,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2020,138 +2020,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="metrics"/>
-      <sheetName val="experiment"/>
-      <sheetName val="survey"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>Strongly Disagree</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>Disagree</v>
-          </cell>
-          <cell r="D2" t="str">
-            <v>Neutral</v>
-          </cell>
-          <cell r="E2" t="str">
-            <v>Agree</v>
-          </cell>
-          <cell r="F2" t="str">
-            <v>Strongly Agree</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Service Orientation</v>
-          </cell>
-          <cell r="B3">
-            <v>0</v>
-          </cell>
-          <cell r="C3">
-            <v>2</v>
-          </cell>
-          <cell r="D3">
-            <v>4</v>
-          </cell>
-          <cell r="E3">
-            <v>20</v>
-          </cell>
-          <cell r="F3">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Object Orientation</v>
-          </cell>
-          <cell r="B4">
-            <v>1</v>
-          </cell>
-          <cell r="C4">
-            <v>7</v>
-          </cell>
-          <cell r="D4">
-            <v>8</v>
-          </cell>
-          <cell r="E4">
-            <v>15</v>
-          </cell>
-          <cell r="F4">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17" t="str">
-            <v>Strongly Disagree</v>
-          </cell>
-          <cell r="C17" t="str">
-            <v>Disagree</v>
-          </cell>
-          <cell r="D17" t="str">
-            <v>Neutral</v>
-          </cell>
-          <cell r="E17" t="str">
-            <v>Agree</v>
-          </cell>
-          <cell r="F17" t="str">
-            <v>Strongly Agree</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>Service Orientation</v>
-          </cell>
-          <cell r="B18">
-            <v>0</v>
-          </cell>
-          <cell r="C18">
-            <v>3</v>
-          </cell>
-          <cell r="D18">
-            <v>4</v>
-          </cell>
-          <cell r="E18">
-            <v>22</v>
-          </cell>
-          <cell r="F18">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>Object Orientation</v>
-          </cell>
-          <cell r="B19">
-            <v>0</v>
-          </cell>
-          <cell r="C19">
-            <v>1</v>
-          </cell>
-          <cell r="D19">
-            <v>12</v>
-          </cell>
-          <cell r="E19">
-            <v>15</v>
-          </cell>
-          <cell r="F19">
-            <v>4</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2453,15 +2321,15 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" thickBot="1">
@@ -2487,7 +2355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1">
+    <row r="2" spans="1:7" thickTop="1">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -2510,7 +2378,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="14.4">
       <c r="A3" s="21" t="s">
         <v>22</v>
       </c>
@@ -2533,7 +2401,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="14.4">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
@@ -2550,7 +2418,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="14.4">
       <c r="A5" s="22"/>
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
@@ -2567,11 +2435,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="14.4">
       <c r="A6" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="26" t="s">
         <v>69</v>
       </c>
       <c r="C6" s="24" t="s">
@@ -2586,11 +2454,11 @@
       <c r="F6" s="3">
         <v>20</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="25" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="14.4">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -2605,7 +2473,7 @@
       </c>
       <c r="G7" s="22"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="14.4">
       <c r="A8" s="21" t="s">
         <v>24</v>
       </c>
@@ -2628,7 +2496,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="14.4">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
@@ -2645,7 +2513,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="14.4">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -2668,7 +2536,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="14.4">
       <c r="A11" s="21" t="s">
         <v>26</v>
       </c>
@@ -2687,11 +2555,11 @@
       <c r="F11" s="3">
         <v>9</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="14.4">
       <c r="A12" s="22"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
@@ -2706,7 +2574,7 @@
       </c>
       <c r="G12" s="22"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="14.4">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
@@ -2723,7 +2591,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="14.4">
       <c r="A14" s="21" t="s">
         <v>27</v>
       </c>
@@ -2746,7 +2614,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" ht="14.4">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
@@ -2763,7 +2631,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" ht="14.4">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
@@ -2786,7 +2654,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" ht="14.4">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
@@ -2809,7 +2677,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" ht="14.4">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
@@ -2832,14 +2700,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" ht="14.4">
       <c r="B19" s="1"/>
       <c r="C19" s="5"/>
       <c r="D19" s="2"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" ht="14.4">
       <c r="B20" s="1"/>
       <c r="C20" s="5"/>
       <c r="D20" s="2"/>
@@ -9708,6 +9576,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
@@ -9719,12 +9593,6 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup scale="45" orientation="landscape"/>
@@ -9742,20 +9610,20 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.85546875" customWidth="1"/>
-    <col min="8" max="8" width="46.28515625" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.88671875" customWidth="1"/>
+    <col min="8" max="8" width="46.33203125" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9800,7 +9668,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" thickTop="1">
+    <row r="2" spans="1:13" thickTop="1">
       <c r="A2" s="13" t="s">
         <v>31</v>
       </c>
@@ -9841,7 +9709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="45">
+    <row r="3" spans="1:13" ht="43.2">
       <c r="A3" s="13" t="s">
         <v>32</v>
       </c>
@@ -9882,7 +9750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30">
+    <row r="4" spans="1:13" ht="14.4">
       <c r="A4" s="13" t="s">
         <v>33</v>
       </c>
@@ -9964,7 +9832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" ht="14.4">
       <c r="A6" s="28" t="s">
         <v>35</v>
       </c>
@@ -10005,7 +9873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" ht="14.4">
       <c r="A7" s="28"/>
       <c r="B7" s="29"/>
       <c r="C7" s="28"/>
@@ -10032,7 +9900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30">
+    <row r="8" spans="1:13" ht="28.8">
       <c r="A8" s="13" t="s">
         <v>36</v>
       </c>
@@ -10073,7 +9941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="45">
+    <row r="9" spans="1:13" ht="28.8">
       <c r="A9" s="13" t="s">
         <v>37</v>
       </c>
@@ -10114,7 +9982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" ht="14.4">
       <c r="A10" s="13" t="s">
         <v>38</v>
       </c>
@@ -10155,7 +10023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" ht="14.4">
       <c r="A11" s="28" t="s">
         <v>39</v>
       </c>
@@ -10196,7 +10064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" ht="14.4">
       <c r="A12" s="28"/>
       <c r="B12" s="29"/>
       <c r="C12" s="28"/>
@@ -10227,7 +10095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" ht="14.4">
       <c r="A13" s="13" t="s">
         <v>40</v>
       </c>
@@ -10268,7 +10136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" ht="14.4">
       <c r="A14" s="28" t="s">
         <v>41</v>
       </c>
@@ -10309,7 +10177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30">
+    <row r="15" spans="1:13" ht="28.8">
       <c r="A15" s="28"/>
       <c r="B15" s="29"/>
       <c r="C15" s="28"/>
@@ -10342,7 +10210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="30">
+    <row r="16" spans="1:13" ht="28.8">
       <c r="A16" s="13" t="s">
         <v>43</v>
       </c>
@@ -10383,7 +10251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" ht="14.4">
       <c r="A17" s="13" t="s">
         <v>44</v>
       </c>
@@ -10424,7 +10292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="30">
+    <row r="18" spans="1:13" ht="28.8">
       <c r="A18" s="4" t="s">
         <v>45</v>
       </c>
@@ -10497,8 +10365,32 @@
         <v>0.76470588235294112</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75" customHeight="1" thickTop="1"/>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="20" spans="1:13" s="16" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A20" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="I20" s="16">
+        <f>MEDIAN(I8:I18)</f>
+        <v>2</v>
+      </c>
+      <c r="J20" s="16">
+        <f t="shared" ref="J20:M20" si="1">MEDIAN(J8:J18)</f>
+        <v>1</v>
+      </c>
+      <c r="K20" s="16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L20" s="16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M20" s="16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" thickTop="1"/>
     <row r="22" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="23" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="24" spans="1:13" ht="15.75" customHeight="1"/>
@@ -11505,14 +11397,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6">

</xml_diff>